<commit_message>
Add to credits + cleaunp
</commit_message>
<xml_diff>
--- a/vars and flags.xlsx
+++ b/vars and flags.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sondr\Dropbox\pokemon_hack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sondr\dev\rocket-edition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE3ADE7-A4C2-445A-B3CE-3395C1E2F85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4282470-C2FE-40EE-8811-F4E8EEEB4F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2845,61 +2845,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>370417</xdr:colOff>
-      <xdr:row>224</xdr:row>
-      <xdr:rowOff>132294</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1127040</xdr:colOff>
-      <xdr:row>235</xdr:row>
-      <xdr:rowOff>96600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Bilde 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5380567" y="39375294"/>
-          <a:ext cx="4259283" cy="2050281"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3199,7 +3144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B183" sqref="B183"/>
     </sheetView>
@@ -7015,7 +6960,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>